<commit_message>
Entrance e DR tested 100% before adding some NullPointerException and other, need to check if NullPointerException is useful, added IllegalArgumentException in Dashboard constructor, added Tower.getID and related Exception when adding Towers in Dashboard
</commit_message>
<xml_diff>
--- a/Development files/Zambo/TestProgress.xlsx
+++ b/Development files/Zambo/TestProgress.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/ae7f41e9afc894df/Desktop/Cartelle/UNI/IngSoft/Progetto/Development files/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matti\OneDrive\Desktop\Cartelle\UNI\IngSoft\Progetto\ProjectFolder\Development files\Zambo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="93" documentId="8_{83C58FEB-6545-4FFD-A8B9-3DD26428D34C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{292DC372-7488-425A-B222-3F4282EB7FDD}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA5506A8-374B-48CA-B45C-73ED16B8D90D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{D15CE968-B1BA-44DA-A95F-CEE23D34429E}"/>
+    <workbookView xWindow="9390" yWindow="1785" windowWidth="12630" windowHeight="11385" xr2:uid="{D15CE968-B1BA-44DA-A95F-CEE23D34429E}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="39">
   <si>
     <t>CLASSE</t>
   </si>
@@ -147,6 +147,12 @@
   </si>
   <si>
     <t>Controllare tutti i metodi necessari in Dashboard rileggendo il regolamento</t>
+  </si>
+  <si>
+    <t>Valutare se è il caso di lanciare NullPointerException quando viene passato un oggetto null nei vari add di Dashboard, Entrance e DiningRoom</t>
+  </si>
+  <si>
+    <t>Altro test su null pointer exception da fare</t>
   </si>
 </sst>
 </file>
@@ -223,7 +229,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -233,9 +239,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -250,11 +253,15 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="13">
+  <dxfs count="3">
     <dxf>
       <fill>
         <patternFill>
@@ -320,96 +327,6 @@
           <color theme="2"/>
         </bottom>
       </border>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF9999"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color theme="2"/>
-        </left>
-        <right style="thin">
-          <color theme="2"/>
-        </right>
-        <top style="thin">
-          <color theme="2"/>
-        </top>
-        <bottom style="thin">
-          <color theme="2"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF99"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF99FF99"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF9999"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF99"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF99FF99"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF7C80"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF9999"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF99"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF99FF99"/>
-        </patternFill>
-      </fill>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -747,8 +664,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB3F9635-3BCD-4CA1-9BD3-FA46FFFB1B2F}">
   <dimension ref="A1:E31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A28" sqref="A28"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -778,7 +695,7 @@
       </c>
     </row>
     <row r="2" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="12" t="s">
         <v>3</v>
       </c>
       <c r="B2" t="s">
@@ -792,7 +709,7 @@
       </c>
     </row>
     <row r="3" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="4"/>
+      <c r="A3" s="12"/>
       <c r="B3" t="s">
         <v>15</v>
       </c>
@@ -801,16 +718,19 @@
       </c>
     </row>
     <row r="4" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="4"/>
+      <c r="A4" s="12"/>
       <c r="B4" t="s">
         <v>16</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>10</v>
+        <v>12</v>
+      </c>
+      <c r="D4" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="4"/>
+      <c r="A5" s="12"/>
       <c r="B5" t="s">
         <v>17</v>
       </c>
@@ -822,19 +742,16 @@
       </c>
     </row>
     <row r="6" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="4"/>
+      <c r="A6" s="12"/>
       <c r="B6" t="s">
         <v>18</v>
       </c>
-      <c r="C6" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="D6" t="s">
-        <v>22</v>
+      <c r="C6" s="9" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="4"/>
+      <c r="A7" s="12"/>
       <c r="B7" t="s">
         <v>19</v>
       </c>
@@ -843,17 +760,21 @@
       </c>
     </row>
     <row r="8" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="4"/>
+      <c r="A8" s="12"/>
       <c r="B8" t="s">
         <v>21</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>38</v>
+      </c>
+    </row>
     <row r="10" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="4" t="s">
+      <c r="A10" s="12" t="s">
         <v>13</v>
       </c>
       <c r="B10" t="s">
@@ -864,7 +785,7 @@
       </c>
     </row>
     <row r="11" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="4"/>
+      <c r="A11" s="12"/>
       <c r="B11" t="s">
         <v>6</v>
       </c>
@@ -873,34 +794,34 @@
       </c>
     </row>
     <row r="12" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="4"/>
+      <c r="A12" s="12"/>
       <c r="B12" t="s">
         <v>7</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="4"/>
+      <c r="A13" s="12"/>
       <c r="B13" t="s">
         <v>8</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="4"/>
+      <c r="A14" s="12"/>
       <c r="B14" t="s">
         <v>9</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="4" t="s">
+      <c r="A16" s="12" t="s">
         <v>23</v>
       </c>
       <c r="B16" t="s">
@@ -911,16 +832,16 @@
       </c>
     </row>
     <row r="17" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="4"/>
+      <c r="A17" s="12"/>
       <c r="B17" t="s">
         <v>26</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="4"/>
+      <c r="A18" s="12"/>
       <c r="B18" t="s">
         <v>28</v>
       </c>
@@ -929,7 +850,7 @@
       </c>
     </row>
     <row r="19" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="4"/>
+      <c r="A19" s="12"/>
       <c r="B19" t="s">
         <v>29</v>
       </c>
@@ -938,7 +859,7 @@
       </c>
     </row>
     <row r="20" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="4"/>
+      <c r="A20" s="12"/>
       <c r="B20" t="s">
         <v>31</v>
       </c>
@@ -947,7 +868,7 @@
       </c>
     </row>
     <row r="21" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="4"/>
+      <c r="A21" s="12"/>
       <c r="B21" t="s">
         <v>30</v>
       </c>
@@ -956,7 +877,7 @@
       </c>
     </row>
     <row r="22" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="4"/>
+      <c r="A22" s="12"/>
       <c r="B22" t="s">
         <v>32</v>
       </c>
@@ -965,7 +886,7 @@
       </c>
     </row>
     <row r="23" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="4"/>
+      <c r="A23" s="12"/>
       <c r="B23" t="s">
         <v>33</v>
       </c>
@@ -974,7 +895,7 @@
       </c>
     </row>
     <row r="24" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="4"/>
+      <c r="A24" s="12"/>
       <c r="B24" t="s">
         <v>34</v>
       </c>
@@ -983,7 +904,7 @@
       </c>
     </row>
     <row r="25" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="4"/>
+      <c r="A25" s="12"/>
       <c r="B25" t="s">
         <v>35</v>
       </c>
@@ -992,7 +913,7 @@
       </c>
     </row>
     <row r="26" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="4"/>
+      <c r="A26" s="12"/>
       <c r="B26" t="s">
         <v>27</v>
       </c>
@@ -1001,11 +922,13 @@
       </c>
     </row>
     <row r="27" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="9"/>
+      <c r="A27" s="8"/>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B28" s="8"/>
-      <c r="C28" s="11"/>
+      <c r="B28" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="C28" s="10"/>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
@@ -1013,7 +936,7 @@
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B31" s="8"/>
+      <c r="B31" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -1140,17 +1063,17 @@
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="6" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="5" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
+      <c r="A4" s="4" t="s">
         <v>12</v>
       </c>
     </row>

</xml_diff>

<commit_message>
NullPointerException added in Entrance methods, tower methods in Dashboard completely tested
</commit_message>
<xml_diff>
--- a/Development files/Zambo/TestProgress.xlsx
+++ b/Development files/Zambo/TestProgress.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matti\OneDrive\Desktop\Cartelle\UNI\IngSoft\Progetto\ProjectFolder\Development files\Zambo\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/ae7f41e9afc894df/Desktop/Cartelle/UNI/IngSoft/Progetto/ProjectFolder/Development files/Zambo/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA5506A8-374B-48CA-B45C-73ED16B8D90D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="20" documentId="13_ncr:1_{BA5506A8-374B-48CA-B45C-73ED16B8D90D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8F211839-A3A4-4251-9865-6D8F891E59F5}"/>
   <bookViews>
-    <workbookView xWindow="9390" yWindow="1785" windowWidth="12630" windowHeight="11385" xr2:uid="{D15CE968-B1BA-44DA-A95F-CEE23D34429E}"/>
+    <workbookView xWindow="-24120" yWindow="2460" windowWidth="24240" windowHeight="13290" xr2:uid="{D15CE968-B1BA-44DA-A95F-CEE23D34429E}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="41">
   <si>
     <t>CLASSE</t>
   </si>
@@ -116,9 +116,6 @@
     <t>BasicTowersMethodTest</t>
   </si>
   <si>
-    <t>TowersMethodExceptionsTest</t>
-  </si>
-  <si>
     <t>KnightParamTest</t>
   </si>
   <si>
@@ -152,7 +149,16 @@
     <t>Valutare se è il caso di lanciare NullPointerException quando viene passato un oggetto null nei vari add di Dashboard, Entrance e DiningRoom</t>
   </si>
   <si>
-    <t>Altro test su null pointer exception da fare</t>
+    <t>NullPointerExceptionTest</t>
+  </si>
+  <si>
+    <t>ConstructorExceptionsTest</t>
+  </si>
+  <si>
+    <t>AddTowersMethodExceptionsTest</t>
+  </si>
+  <si>
+    <t>RemoveTowersMethodExceptionsTest</t>
   </si>
 </sst>
 </file>
@@ -662,10 +668,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB3F9635-3BCD-4CA1-9BD3-FA46FFFB1B2F}">
-  <dimension ref="A1:E31"/>
+  <dimension ref="A1:E34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -769,25 +775,21 @@
       </c>
     </row>
     <row r="9" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="12"/>
       <c r="B9" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="11" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B11" t="s">
         <v>5</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="12"/>
-      <c r="B11" t="s">
-        <v>6</v>
       </c>
       <c r="C11" s="3" t="s">
         <v>10</v>
@@ -796,7 +798,7 @@
     <row r="12" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="12"/>
       <c r="B12" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C12" s="3" t="s">
         <v>10</v>
@@ -805,7 +807,7 @@
     <row r="13" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="12"/>
       <c r="B13" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C13" s="3" t="s">
         <v>10</v>
@@ -814,63 +816,63 @@
     <row r="14" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="12"/>
       <c r="B14" t="s">
+        <v>8</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="12"/>
+      <c r="B15" t="s">
         <v>9</v>
       </c>
-      <c r="C14" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="12" t="s">
+      <c r="C15" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A17" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="B16" t="s">
-        <v>25</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="12"/>
       <c r="B17" t="s">
-        <v>26</v>
+        <v>38</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="12"/>
       <c r="B18" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="12"/>
       <c r="B19" t="s">
-        <v>29</v>
+        <v>39</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="12"/>
       <c r="B20" t="s">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="12"/>
       <c r="B21" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C21" s="3" t="s">
         <v>11</v>
@@ -879,7 +881,7 @@
     <row r="22" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="12"/>
       <c r="B22" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="C22" s="3" t="s">
         <v>11</v>
@@ -888,7 +890,7 @@
     <row r="23" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="12"/>
       <c r="B23" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C23" s="3" t="s">
         <v>11</v>
@@ -897,7 +899,7 @@
     <row r="24" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="12"/>
       <c r="B24" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="C24" s="3" t="s">
         <v>11</v>
@@ -906,7 +908,7 @@
     <row r="25" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="12"/>
       <c r="B25" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="C25" s="3" t="s">
         <v>11</v>
@@ -915,34 +917,61 @@
     <row r="26" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="12"/>
       <c r="B26" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="C26" s="3" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="8"/>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B28" s="11" t="s">
-        <v>37</v>
-      </c>
-      <c r="C28" s="10"/>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" s="12"/>
+      <c r="B27" t="s">
+        <v>33</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="12"/>
+      <c r="B28" t="s">
+        <v>34</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="12"/>
       <c r="B29" t="s">
+        <v>26</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="8"/>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B31" s="11" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B31" s="7"/>
+      <c r="C31" s="10"/>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B32" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="34" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B34" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="3">
-    <mergeCell ref="A2:A8"/>
-    <mergeCell ref="A10:A14"/>
-    <mergeCell ref="A16:A26"/>
+    <mergeCell ref="A11:A15"/>
+    <mergeCell ref="A2:A9"/>
+    <mergeCell ref="A17:A29"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Entrance, DR and Masters tested on Dashboard
</commit_message>
<xml_diff>
--- a/Development files/Zambo/TestProgress.xlsx
+++ b/Development files/Zambo/TestProgress.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/ae7f41e9afc894df/Desktop/Cartelle/UNI/IngSoft/Progetto/ProjectFolder/Development files/Zambo/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="20" documentId="13_ncr:1_{BA5506A8-374B-48CA-B45C-73ED16B8D90D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8F211839-A3A4-4251-9865-6D8F891E59F5}"/>
+  <xr:revisionPtr revIDLastSave="54" documentId="13_ncr:1_{BA5506A8-374B-48CA-B45C-73ED16B8D90D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7D7A8989-E916-4B97-9302-6651E169F6CE}"/>
   <bookViews>
     <workbookView xWindow="-24120" yWindow="2460" windowWidth="24240" windowHeight="13290" xr2:uid="{D15CE968-B1BA-44DA-A95F-CEE23D34429E}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="46">
   <si>
     <t>CLASSE</t>
   </si>
@@ -74,9 +74,6 @@
     <t>TO DO</t>
   </si>
   <si>
-    <t>FAILED</t>
-  </si>
-  <si>
     <t>DR</t>
   </si>
   <si>
@@ -122,9 +119,6 @@
     <t>InsertAndRemoveFromEntranceTest</t>
   </si>
   <si>
-    <t>InsertAndCheckDR</t>
-  </si>
-  <si>
     <t>CardTest</t>
   </si>
   <si>
@@ -159,6 +153,27 @@
   </si>
   <si>
     <t>RemoveTowersMethodExceptionsTest</t>
+  </si>
+  <si>
+    <t>MoveFromEntranceTODRTest</t>
+  </si>
+  <si>
+    <t>ModifyStudentsAlreadyAddedExternally</t>
+  </si>
+  <si>
+    <t>Bisogna controllare che non venga modificato uno studente inserito nella entrance modificando il set usato per inserirlo</t>
+  </si>
+  <si>
+    <t>Molto probabilmente eccezione inutile</t>
+  </si>
+  <si>
+    <t>Usato per controllare che gli studenti vengano inseriti nella DR</t>
+  </si>
+  <si>
+    <t>FAILED/USELESS</t>
+  </si>
+  <si>
+    <t>Bisogna controllare che non venga modificato uno studente inserito nella entrance modificando lo studente passato, inutile, lo studente non può essere modificato</t>
   </si>
 </sst>
 </file>
@@ -668,10 +683,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB3F9635-3BCD-4CA1-9BD3-FA46FFFB1B2F}">
-  <dimension ref="A1:E34"/>
+  <dimension ref="A1:E36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -697,7 +712,7 @@
         <v>2</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -705,19 +720,19 @@
         <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>10</v>
       </c>
       <c r="D2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="12"/>
       <c r="B3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>10</v>
@@ -726,31 +741,31 @@
     <row r="4" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="12"/>
       <c r="B4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>12</v>
+        <v>44</v>
       </c>
       <c r="D4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="12"/>
       <c r="B5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>12</v>
+        <v>44</v>
       </c>
       <c r="D5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="12"/>
       <c r="B6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C6" s="9" t="s">
         <v>10</v>
@@ -759,7 +774,7 @@
     <row r="7" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="12"/>
       <c r="B7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>10</v>
@@ -768,7 +783,7 @@
     <row r="8" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="12"/>
       <c r="B8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>10</v>
@@ -777,28 +792,31 @@
     <row r="9" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="12"/>
       <c r="B9" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="11" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="12" t="s">
-        <v>13</v>
-      </c>
-      <c r="B11" t="s">
+        <v>44</v>
+      </c>
+      <c r="D9" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="12"/>
+      <c r="B10" t="s">
+        <v>35</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="12" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12" t="s">
         <v>5</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="12"/>
-      <c r="B12" t="s">
-        <v>6</v>
       </c>
       <c r="C12" s="3" t="s">
         <v>10</v>
@@ -807,7 +825,7 @@
     <row r="13" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="12"/>
       <c r="B13" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C13" s="3" t="s">
         <v>10</v>
@@ -816,7 +834,7 @@
     <row r="14" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="12"/>
       <c r="B14" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C14" s="3" t="s">
         <v>10</v>
@@ -825,153 +843,180 @@
     <row r="15" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="12"/>
       <c r="B15" t="s">
+        <v>8</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="12"/>
+      <c r="B16" t="s">
         <v>9</v>
       </c>
-      <c r="C15" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="A17" s="12" t="s">
-        <v>23</v>
-      </c>
+      <c r="C16" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="12"/>
       <c r="B17" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="12"/>
-      <c r="B18" t="s">
-        <v>25</v>
-      </c>
-      <c r="C18" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="12"/>
+        <v>44</v>
+      </c>
+      <c r="D17" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A19" s="12" t="s">
+        <v>22</v>
+      </c>
       <c r="B19" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C19" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="12"/>
       <c r="B20" t="s">
-        <v>40</v>
+        <v>24</v>
       </c>
       <c r="C20" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="12"/>
       <c r="B21" t="s">
-        <v>27</v>
+        <v>37</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="12"/>
       <c r="B22" t="s">
-        <v>28</v>
+        <v>38</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="12"/>
       <c r="B23" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="12"/>
       <c r="B24" t="s">
-        <v>29</v>
+        <v>39</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+      <c r="D24" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="12"/>
       <c r="B25" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C25" s="3" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D25" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="12"/>
       <c r="B26" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="12"/>
       <c r="B27" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="12"/>
       <c r="B28" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="C28" s="3" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="12"/>
       <c r="B29" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="C29" s="3" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="8"/>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B31" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="C31" s="10"/>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B32" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="34" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B34" s="7"/>
+    <row r="30" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="12"/>
+      <c r="B30" t="s">
+        <v>32</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="12"/>
+      <c r="B31" t="s">
+        <v>25</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="8"/>
+    </row>
+    <row r="33" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B33" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="C33" s="10"/>
+    </row>
+    <row r="34" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B34" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="36" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B36" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="3">
-    <mergeCell ref="A11:A15"/>
-    <mergeCell ref="A2:A9"/>
-    <mergeCell ref="A17:A29"/>
+    <mergeCell ref="A2:A10"/>
+    <mergeCell ref="A19:A31"/>
+    <mergeCell ref="A12:A17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1079,11 +1124,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05BB0471-34BB-426F-8FD6-1B93490EC0BE}">
   <dimension ref="A1:A4"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.42578125" customWidth="1"/>
+    <col min="1" max="1" width="28.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
@@ -1103,7 +1150,7 @@
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>12</v>
+        <v>44</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Closing connections not perfect but working
</commit_message>
<xml_diff>
--- a/Development files/Zambo/TestProgress.xlsx
+++ b/Development files/Zambo/TestProgress.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/ae7f41e9afc894df/Desktop/Cartelle/UNI/IngSoft/Progetto/ProjectFolder/Development files/Zambo/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\IngSoftProject\ing-sw-2022-Tonsi-Zambetti-Vaia\Development files\Zambo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="54" documentId="13_ncr:1_{BA5506A8-374B-48CA-B45C-73ED16B8D90D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7D7A8989-E916-4B97-9302-6651E169F6CE}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7C93AD6-2E9E-4E97-8105-5A4C090BBCCA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-24120" yWindow="2460" windowWidth="24240" windowHeight="13290" xr2:uid="{D15CE968-B1BA-44DA-A95F-CEE23D34429E}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13260" xr2:uid="{D15CE968-B1BA-44DA-A95F-CEE23D34429E}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="57">
   <si>
     <t>CLASSE</t>
   </si>
@@ -174,6 +174,39 @@
   </si>
   <si>
     <t>Bisogna controllare che non venga modificato uno studente inserito nella entrance modificando lo studente passato, inutile, lo studente non può essere modificato</t>
+  </si>
+  <si>
+    <t>Chiusura connessioni</t>
+  </si>
+  <si>
+    <t>Partita finita</t>
+  </si>
+  <si>
+    <t>Partita in fase di creazione sul primo client, gli altri in attesa, si disconnette il client che crea la partita</t>
+  </si>
+  <si>
+    <t>Partita in fase di creazione sul primo client, gli altri in attesa, si disconnettono gli altri client</t>
+  </si>
+  <si>
+    <t>I client in partita vengono correttamente disconnessi</t>
+  </si>
+  <si>
+    <t>Partita iniziata, altri client si collegano e disconnettono</t>
+  </si>
+  <si>
+    <t>Viene segnalato che la lobby è piena</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tutti gli altri </t>
+  </si>
+  <si>
+    <t>Parametri partita settati, un client qualsiasi in partita si disconnette (uguale a partita iniziata), 2 giocatori</t>
+  </si>
+  <si>
+    <t>Parametri partita settati, un client qualsiasi in partita si disconnette (uguale a partita iniziata), 3 giocatori</t>
+  </si>
+  <si>
+    <t>Funziona correttamente ma viene lanciata un'eccezione quando si prova a chiudere l'ObjectOutputStream</t>
   </si>
 </sst>
 </file>
@@ -264,7 +297,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -277,6 +309,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -683,10 +718,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB3F9635-3BCD-4CA1-9BD3-FA46FFFB1B2F}">
-  <dimension ref="A1:E36"/>
+  <dimension ref="A1:E41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="B43" sqref="B43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -716,7 +751,7 @@
       </c>
     </row>
     <row r="2" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="12" t="s">
+      <c r="A2" s="11" t="s">
         <v>3</v>
       </c>
       <c r="B2" t="s">
@@ -730,7 +765,7 @@
       </c>
     </row>
     <row r="3" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="12"/>
+      <c r="A3" s="11"/>
       <c r="B3" t="s">
         <v>14</v>
       </c>
@@ -739,7 +774,7 @@
       </c>
     </row>
     <row r="4" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="12"/>
+      <c r="A4" s="11"/>
       <c r="B4" t="s">
         <v>15</v>
       </c>
@@ -751,7 +786,7 @@
       </c>
     </row>
     <row r="5" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="12"/>
+      <c r="A5" s="11"/>
       <c r="B5" t="s">
         <v>16</v>
       </c>
@@ -763,16 +798,16 @@
       </c>
     </row>
     <row r="6" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="12"/>
+      <c r="A6" s="11"/>
       <c r="B6" t="s">
         <v>17</v>
       </c>
-      <c r="C6" s="9" t="s">
+      <c r="C6" s="8" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="12"/>
+      <c r="A7" s="11"/>
       <c r="B7" t="s">
         <v>18</v>
       </c>
@@ -781,7 +816,7 @@
       </c>
     </row>
     <row r="8" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="12"/>
+      <c r="A8" s="11"/>
       <c r="B8" t="s">
         <v>20</v>
       </c>
@@ -790,7 +825,7 @@
       </c>
     </row>
     <row r="9" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="12"/>
+      <c r="A9" s="11"/>
       <c r="B9" t="s">
         <v>40</v>
       </c>
@@ -802,7 +837,7 @@
       </c>
     </row>
     <row r="10" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="12"/>
+      <c r="A10" s="11"/>
       <c r="B10" t="s">
         <v>35</v>
       </c>
@@ -812,7 +847,7 @@
     </row>
     <row r="11" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="12" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="12" t="s">
+      <c r="A12" s="11" t="s">
         <v>12</v>
       </c>
       <c r="B12" t="s">
@@ -823,7 +858,7 @@
       </c>
     </row>
     <row r="13" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="12"/>
+      <c r="A13" s="11"/>
       <c r="B13" t="s">
         <v>6</v>
       </c>
@@ -832,7 +867,7 @@
       </c>
     </row>
     <row r="14" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="12"/>
+      <c r="A14" s="11"/>
       <c r="B14" t="s">
         <v>7</v>
       </c>
@@ -841,7 +876,7 @@
       </c>
     </row>
     <row r="15" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="12"/>
+      <c r="A15" s="11"/>
       <c r="B15" t="s">
         <v>8</v>
       </c>
@@ -850,7 +885,7 @@
       </c>
     </row>
     <row r="16" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="12"/>
+      <c r="A16" s="11"/>
       <c r="B16" t="s">
         <v>9</v>
       </c>
@@ -859,7 +894,7 @@
       </c>
     </row>
     <row r="17" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="12"/>
+      <c r="A17" s="11"/>
       <c r="B17" t="s">
         <v>40</v>
       </c>
@@ -871,7 +906,7 @@
       </c>
     </row>
     <row r="19" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A19" s="12" t="s">
+      <c r="A19" s="11" t="s">
         <v>22</v>
       </c>
       <c r="B19" t="s">
@@ -882,7 +917,7 @@
       </c>
     </row>
     <row r="20" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="12"/>
+      <c r="A20" s="11"/>
       <c r="B20" t="s">
         <v>24</v>
       </c>
@@ -891,7 +926,7 @@
       </c>
     </row>
     <row r="21" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="12"/>
+      <c r="A21" s="11"/>
       <c r="B21" t="s">
         <v>37</v>
       </c>
@@ -900,7 +935,7 @@
       </c>
     </row>
     <row r="22" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="12"/>
+      <c r="A22" s="11"/>
       <c r="B22" t="s">
         <v>38</v>
       </c>
@@ -909,7 +944,7 @@
       </c>
     </row>
     <row r="23" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="12"/>
+      <c r="A23" s="11"/>
       <c r="B23" t="s">
         <v>26</v>
       </c>
@@ -918,7 +953,7 @@
       </c>
     </row>
     <row r="24" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="12"/>
+      <c r="A24" s="11"/>
       <c r="B24" t="s">
         <v>39</v>
       </c>
@@ -930,7 +965,7 @@
       </c>
     </row>
     <row r="25" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="12"/>
+      <c r="A25" s="11"/>
       <c r="B25" t="s">
         <v>28</v>
       </c>
@@ -942,7 +977,7 @@
       </c>
     </row>
     <row r="26" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="12"/>
+      <c r="A26" s="11"/>
       <c r="B26" t="s">
         <v>27</v>
       </c>
@@ -951,7 +986,7 @@
       </c>
     </row>
     <row r="27" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="12"/>
+      <c r="A27" s="11"/>
       <c r="B27" t="s">
         <v>29</v>
       </c>
@@ -960,7 +995,7 @@
       </c>
     </row>
     <row r="28" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="12"/>
+      <c r="A28" s="11"/>
       <c r="B28" t="s">
         <v>30</v>
       </c>
@@ -969,7 +1004,7 @@
       </c>
     </row>
     <row r="29" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="12"/>
+      <c r="A29" s="11"/>
       <c r="B29" t="s">
         <v>31</v>
       </c>
@@ -978,7 +1013,7 @@
       </c>
     </row>
     <row r="30" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="12"/>
+      <c r="A30" s="11"/>
       <c r="B30" t="s">
         <v>32</v>
       </c>
@@ -987,7 +1022,7 @@
       </c>
     </row>
     <row r="31" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="12"/>
+      <c r="A31" s="11"/>
       <c r="B31" t="s">
         <v>25</v>
       </c>
@@ -996,27 +1031,96 @@
       </c>
     </row>
     <row r="32" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="8"/>
-    </row>
-    <row r="33" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B33" s="11" t="s">
+      <c r="A32" s="7"/>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B33" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="C33" s="10"/>
-    </row>
-    <row r="34" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C33" s="9"/>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="36" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B36" s="7"/>
+    <row r="36" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="B36" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="C36" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D36" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="11"/>
+      <c r="B37" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="C37" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D37" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="11"/>
+      <c r="B38" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="C38" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="11"/>
+      <c r="B39" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="C39" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="D39" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="11"/>
+      <c r="B40" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="C40" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D40" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="11"/>
+      <c r="B41" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="C41" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D41" t="s">
+        <v>50</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="4">
     <mergeCell ref="A2:A10"/>
     <mergeCell ref="A19:A31"/>
     <mergeCell ref="A12:A17"/>
+    <mergeCell ref="A36:A41"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>